<commit_message>
tdf#141309 tdf#142215 sc fix ooxml autofilter import issues
No need to convert the filter values from sting to number and back,
at ooxml import, because we do that later in the model,
by filtering with the formatted cell vales.

Change-Id: I75e5b2391624ff85a8ed545926ec519355a356bc
</commit_message>
<xml_diff>
--- a/sc/qa/uitest/data/autofilter/tdf140968.xlsx
+++ b/sc/qa/uitest/data/autofilter/tdf140968.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Munka1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Munka1!$A$1:$B$7</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Munka1!$A$1:$B$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t xml:space="preserve">Values</t>
   </si>
@@ -120,15 +120,15 @@
       <charset val="238"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -312,11 +312,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -386,15 +386,15 @@
     <cellStyle name="Error 9" xfId="25"/>
     <cellStyle name="Footnote 10" xfId="26"/>
     <cellStyle name="Good 11" xfId="27"/>
-    <cellStyle name="Heading" xfId="28"/>
-    <cellStyle name="Heading 1 13" xfId="29"/>
-    <cellStyle name="Heading 12" xfId="30"/>
-    <cellStyle name="Heading 2 14" xfId="31"/>
+    <cellStyle name="Heading 1 13" xfId="28"/>
+    <cellStyle name="Heading 12" xfId="29"/>
+    <cellStyle name="Heading 2 14" xfId="30"/>
+    <cellStyle name="Heading 3" xfId="31"/>
     <cellStyle name="Hyperlink 15" xfId="32"/>
     <cellStyle name="Neutral 16" xfId="33"/>
     <cellStyle name="Note 17" xfId="34"/>
-    <cellStyle name="Result" xfId="35"/>
-    <cellStyle name="Result 18" xfId="36"/>
+    <cellStyle name="Result 18" xfId="35"/>
+    <cellStyle name="Result 4" xfId="36"/>
     <cellStyle name="Status 19" xfId="37"/>
     <cellStyle name="Text 20" xfId="38"/>
     <cellStyle name="Warning 21" xfId="39"/>
@@ -471,19 +471,19 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="8.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -491,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0.364849537037037</v>
       </c>
@@ -499,7 +499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>0.0458680555555556</v>
       </c>
@@ -507,7 +507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>0.0458796296296296</v>
       </c>
@@ -515,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0.0458912037037037</v>
       </c>
@@ -523,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>0</v>
       </c>
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>0.516030092592593</v>
       </c>
@@ -539,11 +539,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B7">
+  <autoFilter ref="A1:B8">
     <filterColumn colId="0">
       <filters>
         <filter val="0.046"/>
+        <filter val="0.500"/>
         <filter val="0.516"/>
       </filters>
     </filterColumn>

</xml_diff>